<commit_message>
Adding Unit 1.4 solutions
</commit_message>
<xml_diff>
--- a/01-Class-Activities/01-Excel/4/Activities/01-Ins_CentralTendency/Solved/CentralTendency.xlsx
+++ b/01-Class-Activities/01-Excel/4/Activities/01-Ins_CentralTendency/Solved/CentralTendency.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arwenshackelford/curriculum/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/2/Activities/05-Ins_CentralTendency/Solved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98452\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\4\Activities\01-Ins_CentralTendency\Solved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D80524A-22F4-C741-8E8E-9231F75A930F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Mean Example" sheetId="1" r:id="rId1"/>
     <sheet name="Median Example" sheetId="3" r:id="rId2"/>
     <sheet name="Single-Mode Example" sheetId="6" r:id="rId3"/>
     <sheet name="Multi-Mode Example" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Mean Example'!$A$2:$A$31</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'Median Example'!$A$2:$A$31</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Single-Mode Example'!$A$2:$A$31</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Multi-Mode Example'!$A$2:$A$31</definedName>
+    <definedName name="Nums">'Median Example'!$A$2:$A$31</definedName>
+    <definedName name="SampleNumbers">'Mean Example'!$A$2:$A$31</definedName>
+    <definedName name="SAMPLENUMS">'Multi-Mode Example'!$A$2:$A$31</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="61" r:id="rId6"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,14 +54,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -70,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Sum of Values:</t>
   </si>
@@ -110,11 +116,20 @@
   <si>
     <t>Excel Single-Mode Function:</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Data Set</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -196,7 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -214,6 +229,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -244,7 +263,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{6412C7B8-3504-404F-9303-75E25BB0CFD4}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -258,6 +277,393 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[CentralTendency.xlsx]Sheet1!PivotTable29</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C352-48C8-93B6-B99A5E390982}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="764937407"/>
+        <c:axId val="764941151"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="764937407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="764941151"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="764941151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="764937407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -301,6 +707,9 @@
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="clusteredColumn" uniqueId="{F0E5C7BB-5E50-CF4D-9206-00CEF1898C9B}">
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:binning intervalClosed="r">
@@ -347,6 +756,7 @@
       </cx:axis>
     </cx:plotArea>
   </cx:chart>
+  <cx:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
 </cx:chartSpace>
 </file>
 
@@ -399,8 +809,8 @@
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0"/>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="0.389999986"/>
         <cx:tickLabels/>
         <cx:txPr>
           <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
@@ -780,6 +1190,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -2808,6 +3258,509 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2817,15 +3770,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1562100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>4233</xdr:rowOff>
+      <xdr:colOff>947628</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2502</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1282700</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>21167</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>606136</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19436</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -2840,10 +3793,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3136900" y="2146300"/>
-          <a:ext cx="4572000" cy="2743200"/>
-          <a:chOff x="3136900" y="2146300"/>
-          <a:chExt cx="4572000" cy="2743200"/>
+          <a:off x="2333083" y="1907502"/>
+          <a:ext cx="5304235" cy="2683934"/>
+          <a:chOff x="3454400" y="2056028"/>
+          <a:chExt cx="5896076" cy="2743200"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2860,7 +3813,7 @@
               <xdr:cNvGraphicFramePr/>
             </xdr:nvGraphicFramePr>
             <xdr:xfrm>
-              <a:off x="3136900" y="2146300"/>
+              <a:off x="4778476" y="2056028"/>
               <a:ext cx="4572000" cy="2743200"/>
             </xdr:xfrm>
             <a:graphic>
@@ -2879,10 +3832,6 @@
               </xdr:cNvSpPr>
             </xdr:nvSpPr>
             <xdr:spPr>
-              <a:xfrm>
-                <a:off x="3136900" y="2146300"/>
-                <a:ext cx="4572000" cy="2743200"/>
-              </a:xfrm>
               <a:prstGeom prst="rect">
                 <a:avLst/>
               </a:prstGeom>
@@ -3035,141 +3984,65 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>25401</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="4" name="Group 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D21F88F-F871-7D43-8927-2B63695EAA23}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="4851400" y="2150534"/>
-          <a:ext cx="4572000" cy="2743200"/>
-          <a:chOff x="3136900" y="2146300"/>
-          <a:chExt cx="4572000" cy="2743200"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-          <xdr:graphicFrame macro="">
-            <xdr:nvGraphicFramePr>
-              <xdr:cNvPr id="5" name="Chart 4">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16457FA3-FD94-3245-8C60-3815B8C7C051}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvGraphicFramePr/>
-            </xdr:nvGraphicFramePr>
-            <xdr:xfrm>
-              <a:off x="3136900" y="2146300"/>
-              <a:ext cx="4572000" cy="2743200"/>
-            </xdr:xfrm>
-            <a:graphic>
-              <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-                <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-              </a:graphicData>
-            </a:graphic>
-          </xdr:graphicFrame>
-        </mc:Choice>
-        <mc:Fallback>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="0" name=""/>
-              <xdr:cNvSpPr>
-                <a:spLocks noTextEdit="1"/>
-              </xdr:cNvSpPr>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="3136900" y="2146300"/>
-                <a:ext cx="4572000" cy="2743200"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Chart 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16457FA3-FD94-3245-8C60-3815B8C7C051}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
               <a:solidFill>
-                <a:prstClr val="white"/>
+                <a:prstClr val="green"/>
               </a:solidFill>
-              <a:ln w="1">
-                <a:solidFill>
-                  <a:prstClr val="green"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
-                  <a:t>This chart isn't available in your version of Excel.
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </mc:Fallback>
-      </mc:AlternateContent>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="TextBox 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{464D515A-6F00-1449-802F-1692AA4F1C6D}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3454400" y="4453464"/>
-            <a:ext cx="4165600" cy="330200"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="900" baseline="0"/>
-              <a:t>  1              2              3              4              5              6              7              8              9             10     </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="900"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3180,15 +4053,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1693333</xdr:colOff>
+      <xdr:colOff>1445683</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:rowOff>126999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1168400</xdr:colOff>
+      <xdr:colOff>1130300</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>169332</xdr:rowOff>
+      <xdr:rowOff>143932</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3203,8 +4076,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3268133" y="3852332"/>
-          <a:ext cx="4572000" cy="2743200"/>
+          <a:off x="2829983" y="3746499"/>
+          <a:ext cx="4148667" cy="2683933"/>
           <a:chOff x="3136900" y="2146300"/>
           <a:chExt cx="4572000" cy="2743200"/>
         </a:xfrm>
@@ -3242,10 +4115,6 @@
               </xdr:cNvSpPr>
             </xdr:nvSpPr>
             <xdr:spPr>
-              <a:xfrm>
-                <a:off x="3136900" y="2146300"/>
-                <a:ext cx="4572000" cy="2743200"/>
-              </a:xfrm>
               <a:prstGeom prst="rect">
                 <a:avLst/>
               </a:prstGeom>
@@ -3358,8 +4227,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3293534" y="4648199"/>
-          <a:ext cx="4572000" cy="2743200"/>
+          <a:off x="2887134" y="4550832"/>
+          <a:ext cx="4155017" cy="2683934"/>
           <a:chOff x="3136900" y="2146300"/>
           <a:chExt cx="4572000" cy="2743200"/>
         </a:xfrm>
@@ -3397,10 +4266,6 @@
               </xdr:cNvSpPr>
             </xdr:nvSpPr>
             <xdr:spPr>
-              <a:xfrm>
-                <a:off x="3136900" y="2146300"/>
-                <a:ext cx="4572000" cy="2743200"/>
-              </a:xfrm>
               <a:prstGeom prst="rect">
                 <a:avLst/>
               </a:prstGeom>
@@ -3483,6 +4348,244 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Williams, Dartanion" refreshedDate="44103.84006736111" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="30">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:A31" sheet="Multi-Mode Example"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="Data Set" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="9" count="9">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+        <n v="8"/>
+        <n v="9"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="30">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable29" cacheId="61" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Data Set" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3781,309 +4884,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="14" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="3">
-        <f>SUM(A2:A31)</f>
+      <c r="C6" s="3">
+        <f>SUM(SampleNumbers)</f>
         <v>157</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3">
-        <f>COUNT(A2:A31)</f>
+      <c r="C7" s="3">
+        <f>COUNT(SampleNumbers)</f>
         <v>30</v>
       </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3">
-        <f>D6/D7</f>
+      <c r="C8" s="3">
+        <f>C6/C7</f>
         <v>5.2333333333333334</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3">
-        <f>AVERAGE(A2:A31)</f>
+      <c r="C9" s="3">
+        <f>AVERAGE(SampleNumbers)</f>
         <v>5.2333333333333334</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
@@ -4095,20 +5168,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDF04A9-084C-844B-8575-F334579C420A}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="14" width="20.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="14" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -4119,7 +5194,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -4130,7 +5205,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -4141,7 +5216,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -4152,7 +5227,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4163,7 +5238,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4174,7 +5249,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4189,7 +5264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -4205,7 +5280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -4216,7 +5291,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -4227,7 +5302,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -4238,7 +5313,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -4249,7 +5324,7 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -4260,7 +5335,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -4271,7 +5346,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -4282,7 +5357,7 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -4293,7 +5368,7 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4304,7 +5379,7 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -4315,7 +5390,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -4326,7 +5401,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -4337,7 +5412,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -4348,7 +5423,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
@@ -4359,7 +5434,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -4370,7 +5445,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -4381,7 +5456,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -4392,7 +5467,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -4403,7 +5478,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
@@ -4414,7 +5489,7 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -4425,7 +5500,7 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
@@ -4436,7 +5511,7 @@
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -4447,7 +5522,7 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
@@ -4455,8 +5530,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>MEDIAN(Nums)</f>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B31">
+  <sortState ref="B2:B31">
     <sortCondition ref="B2:B31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4465,20 +5546,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0812124F-9E5E-8045-AC7B-048D697B08A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -4486,7 +5569,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4494,7 +5577,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4502,7 +5585,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4510,7 +5593,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4522,7 +5605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4535,7 +5618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4548,7 +5631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -4561,7 +5644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -4574,7 +5657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -4587,7 +5670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -4600,7 +5683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -4613,7 +5696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -4626,7 +5709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -4639,7 +5722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -4652,7 +5735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -4660,7 +5743,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -4673,7 +5756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -4681,13 +5764,13 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -4695,7 +5778,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -4703,7 +5786,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -4711,7 +5794,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
@@ -4719,7 +5802,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8</v>
       </c>
@@ -4727,7 +5810,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8</v>
       </c>
@@ -4735,7 +5818,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8</v>
       </c>
@@ -4743,7 +5826,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8</v>
       </c>
@@ -4751,7 +5834,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -4759,7 +5842,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9</v>
       </c>
@@ -4767,7 +5850,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10</v>
       </c>
@@ -4775,13 +5858,13 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C6:D15">
+  <sortState ref="C6:D15">
     <sortCondition ref="C6:C15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4790,22 +5873,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5EDFE5C-0ABF-A44C-A15C-1A9152000E71}">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -4813,7 +5894,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4821,7 +5902,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4829,7 +5910,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4837,7 +5918,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4849,7 +5930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4859,10 +5940,10 @@
       </c>
       <c r="D6">
         <f>COUNTIF(A$2:A$31,"=1")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4875,7 +5956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -4885,12 +5966,12 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIF(A$2:A$31,"=3")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="3">
@@ -4901,7 +5982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -4914,7 +5995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -4927,7 +6008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -4940,7 +6021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -4953,7 +6034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -4963,10 +6044,10 @@
       </c>
       <c r="D14" s="8">
         <f>COUNTIF(A$2:A$31,"=9")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -4976,10 +6057,10 @@
       </c>
       <c r="D15" s="8">
         <f>COUNTIF(A$2:A$31,"=10")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -4987,7 +6068,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -4995,7 +6076,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -5003,7 +6084,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -5013,10 +6094,10 @@
       </c>
       <c r="D19" s="3">
         <f>_xlfn.MODE.SNGL(A2:A31)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -5026,46 +6107,62 @@
       </c>
       <c r="D20" cm="1">
         <f t="array" ref="D20:D22">_xlfn.MODE.MULT(A2:A31)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <f t="array" ref="E20:E24">_xlfn.MODE.MULT(SAMPLENUMS)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8</v>
       </c>
@@ -5073,7 +6170,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8</v>
       </c>
@@ -5081,7 +6178,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8</v>
       </c>
@@ -5089,7 +6186,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -5097,7 +6194,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9</v>
       </c>
@@ -5105,24 +6202,133 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C6:D15">
+  <sortState ref="C6:D15">
     <sortCondition ref="C6:C15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>